<commit_message>
Add hip joint to muscle force analysis
Beginning calculations of muscle length/attachment points to move damped hind leg through required range of motion
</commit_message>
<xml_diff>
--- a/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Actuator Pressures Required to Move Joint Springs2.xlsx
+++ b/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Actuator Pressures Required to Move Joint Springs2.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haonan\Documents\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD2D9D7-547C-47A0-90B5-9F1A0803CE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="124">
   <si>
     <t>me</t>
   </si>
@@ -375,12 +381,39 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>hip extensor</t>
+  </si>
+  <si>
+    <t>hip flexor</t>
+  </si>
+  <si>
+    <t>rotation radius hip flexor</t>
+  </si>
+  <si>
+    <t>rotation radius hip extensor</t>
+  </si>
+  <si>
+    <t>torque from hip spring</t>
+  </si>
+  <si>
+    <t>total hip extensor torque</t>
+  </si>
+  <si>
+    <t>total hip flexor torque</t>
+  </si>
+  <si>
+    <t>hip extensor force required</t>
+  </si>
+  <si>
+    <t>hip flexor force required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -526,7 +559,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -852,21 +884,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="14" topLeftCell="Q18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,31 +912,45 @@
     <col min="16" max="16" width="13.140625" customWidth="1"/>
     <col min="19" max="19" width="35.85546875" customWidth="1"/>
     <col min="20" max="20" width="13.140625" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" customWidth="1"/>
+    <col min="27" max="27" width="35.85546875" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G1" s="15" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17"/>
-      <c r="K1" s="15" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="K1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17"/>
-      <c r="O1" s="15" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="O1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="17"/>
-      <c r="S1" s="15" t="s">
+      <c r="P1" s="15"/>
+      <c r="Q1" s="16"/>
+      <c r="S1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="17"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T1" s="15"/>
+      <c r="U1" s="16"/>
+      <c r="W1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="16"/>
+      <c r="AA1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="16"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -917,44 +963,62 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="H2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="L2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="P2">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="T2">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -967,40 +1031,56 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="1">
         <f>H2*2*PI()/360</f>
-        <v>0.715584993317675</v>
+        <v>0.89011791851710798</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="1">
         <f>L2*2*PI()/360</f>
-        <v>0.715584993317675</v>
+        <v>0.75049157835756164</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="18"/>
+      <c r="O3" s="17"/>
       <c r="P3" s="1">
         <f>P2*2*PI()/360</f>
-        <v>0.90757121103705141</v>
+        <v>1.2217304763960306</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="18"/>
+      <c r="S3" s="17"/>
       <c r="T3" s="1">
         <f>T2*2*PI()/360</f>
-        <v>0.31415926535897931</v>
+        <v>0.17453292519943295</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W3" s="17"/>
+      <c r="X3" s="1">
+        <f>X2*2*PI()/360</f>
+        <v>0.87266462599716477</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="1">
+        <f>AB2*2*PI()/360</f>
+        <v>0.87266462599716477</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1013,20 +1093,26 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="1"/>
       <c r="I4" s="4"/>
-      <c r="K4" s="14"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="1"/>
       <c r="M4" s="4"/>
-      <c r="O4" s="14"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="4"/>
-      <c r="S4" s="14"/>
+      <c r="S4" s="13"/>
       <c r="T4" s="1"/>
       <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W4" s="13"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="4"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="4"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1043,8 +1129,8 @@
         <v>113</v>
       </c>
       <c r="H5" s="1">
-        <f>(H3*C39)*1000</f>
-        <v>11.506606692548214</v>
+        <f>(H3*C41)*1000</f>
+        <v>14.313096129755097</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>114</v>
@@ -1053,8 +1139,8 @@
         <v>113</v>
       </c>
       <c r="L5" s="1">
-        <f>(L3*C38)*1000</f>
-        <v>14.769674262076812</v>
+        <f>(L3*C40)*1000</f>
+        <v>15.490146177300073</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>114</v>
@@ -1063,8 +1149,8 @@
         <v>113</v>
       </c>
       <c r="P5" s="1">
-        <f>($C37*P3)*1000</f>
-        <v>23.188444441996666</v>
+        <f>($C39*P3)*1000</f>
+        <v>31.215213671918583</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>114</v>
@@ -1073,20 +1159,40 @@
         <v>113</v>
       </c>
       <c r="T5" s="1">
-        <f>($C36*T3)*1000</f>
-        <v>6.8643799480936982</v>
+        <f>($C38*T3)*1000</f>
+        <v>3.8135444156076104</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="X5" s="1">
+        <f>($C37*X3)*1000</f>
+        <v>6.9267754688524956</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>($C36*AB3)*1000</f>
+        <v>6.9267754688524956</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H6" s="1">
         <f>H5/1000/$C26</f>
-        <v>0.12293383218534418</v>
+        <v>0.15291769369396471</v>
       </c>
       <c r="I6" s="4"/>
       <c r="K6" s="5" t="s">
@@ -1094,7 +1200,7 @@
       </c>
       <c r="L6" s="1">
         <f>L5/1000/$C25</f>
-        <v>0.11949574645693214</v>
+        <v>0.12532480725970932</v>
       </c>
       <c r="M6" s="4"/>
       <c r="O6" s="5" t="s">
@@ -1102,7 +1208,7 @@
       </c>
       <c r="P6" s="1">
         <f>P5/1000/$C24</f>
-        <v>0.14807435786715623</v>
+        <v>0.19933086635963335</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="S6" s="5" t="s">
@@ -1110,11 +1216,27 @@
       </c>
       <c r="T6" s="1">
         <f>T5/1000/$C23</f>
-        <v>4.3281084162003144E-2</v>
+        <v>2.4045046756668412E-2</v>
       </c>
       <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="X6" s="1">
+        <f>X5/1000/$C24</f>
+        <v>4.423228268743612E-2</v>
+      </c>
+      <c r="Y6" s="4"/>
+      <c r="AA6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB6" s="1">
+        <f>AB5/1000/$C23</f>
+        <v>4.3674498542575636E-2</v>
+      </c>
+      <c r="AC6" s="4"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1160,8 +1282,24 @@
         <v>0.16669999999999999</v>
       </c>
       <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="X7" s="1">
+        <f>$C$28</f>
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Y7" s="4"/>
+      <c r="AA7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB7" s="1">
+        <f>$C$28</f>
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AC7" s="4"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G8" s="6"/>
       <c r="I8" s="4"/>
       <c r="K8" s="6"/>
@@ -1170,8 +1308,12 @@
       <c r="Q8" s="4"/>
       <c r="S8" s="6"/>
       <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W8" s="6"/>
+      <c r="Y8" s="4"/>
+      <c r="AA8" s="6"/>
+      <c r="AC8" s="4"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1209,14 +1351,34 @@
         <v>34</v>
       </c>
       <c r="T9">
-        <f>($C16/2)*$C5*$C$7</f>
-        <v>3.4452720000000006E-2</v>
+        <f>(C5*C7)*(C15+(C16/2))+(C2*C15)+(C4+(C30*(C18+C19)))*(C15/2)</f>
+        <v>0.21963739499999999</v>
       </c>
       <c r="U9" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9">
+        <f>(C5*C7)*(C15+(C16/2))+(C2*C15)+(C4+(C30*(C18+C19)))*(C15/2)</f>
+        <v>0.21963739499999999</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB9">
+        <f>(C5*C7)*(C15+(C16/2))+(C2*C15)+(C4+(C30*(C18+C19)))*(C15/2)</f>
+        <v>0.21963739499999999</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1393,7 @@
       </c>
       <c r="H10">
         <f>$C32*H3</f>
-        <v>0.33824987049133182</v>
+        <v>0.42074983890385176</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>54</v>
@@ -1241,7 +1403,7 @@
       </c>
       <c r="L10">
         <f>$C32*L3</f>
-        <v>0.33824987049133182</v>
+        <v>0.3547498641738358</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>54</v>
@@ -1251,7 +1413,7 @@
       </c>
       <c r="P10">
         <f>$C33*P3</f>
-        <v>2.0191126987562029</v>
+        <v>2.7180363252487343</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>54</v>
@@ -1261,13 +1423,33 @@
       </c>
       <c r="T10">
         <f>$C32*T3</f>
-        <v>0.14849994314253592</v>
+        <v>8.2499968412519956E-2</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="X10">
+        <f>$C34*X3</f>
+        <v>34.906585039886593</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB10">
+        <f>$C34*AB3</f>
+        <v>34.906585039886593</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1282,7 +1464,7 @@
       </c>
       <c r="H11">
         <f>SUM(H9:H10)</f>
-        <v>0.37270259049133181</v>
+        <v>0.45520255890385175</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>54</v>
@@ -1292,7 +1474,7 @@
       </c>
       <c r="L11">
         <f>SUM(L9:L10)</f>
-        <v>0.37270259049133181</v>
+        <v>0.3892025841738358</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>54</v>
@@ -1302,7 +1484,7 @@
       </c>
       <c r="P11">
         <f>SUM(P9:P10)</f>
-        <v>2.2387500937562028</v>
+        <v>2.9376737202487342</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>54</v>
@@ -1312,13 +1494,33 @@
       </c>
       <c r="T11">
         <f>SUM(T9:T10)</f>
-        <v>0.18295266314253594</v>
+        <v>0.30213736341251995</v>
       </c>
       <c r="U11" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="X11">
+        <f>SUM(X9:X10)</f>
+        <v>35.126222434886593</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB11">
+        <f>SUM(AB9:AB10)</f>
+        <v>35.126222434886593</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1336,14 +1538,18 @@
       <c r="Q12" s="4"/>
       <c r="S12" s="6"/>
       <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W12" s="6"/>
+      <c r="Y12" s="4"/>
+      <c r="AA12" s="6"/>
+      <c r="AC12" s="4"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G13" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H13">
-        <f>H11/$C39</f>
-        <v>23.178021796724614</v>
+        <f>H11/$C41</f>
+        <v>28.308616847254463</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>57</v>
@@ -1352,8 +1558,8 @@
         <v>56</v>
       </c>
       <c r="L13">
-        <f>L11/$C38</f>
-        <v>18.057296050936621</v>
+        <f>L11/$C40</f>
+        <v>18.856714349507548</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>57</v>
@@ -1362,8 +1568,8 @@
         <v>78</v>
       </c>
       <c r="P13">
-        <f>P11/$C37</f>
-        <v>87.622312867170365</v>
+        <f>P11/$C39</f>
+        <v>114.97744501951993</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>57</v>
@@ -1372,14 +1578,34 @@
         <v>81</v>
       </c>
       <c r="T13">
-        <f>T11/$C39</f>
-        <v>11.377653180505966</v>
+        <f>T11/$C38</f>
+        <v>13.827796952518074</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="X13">
+        <f>X11/$C36</f>
+        <v>4425.3508579384679</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB13">
+        <f>AB11/$C37</f>
+        <v>4425.3508579384679</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1400,8 +1626,12 @@
       <c r="Q14" s="4"/>
       <c r="S14" s="6"/>
       <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W14" s="6"/>
+      <c r="Y14" s="4"/>
+      <c r="AA14" s="6"/>
+      <c r="AC14" s="4"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1418,8 +1648,8 @@
         <v>69</v>
       </c>
       <c r="H15" s="8">
-        <f>($C$42+$C$43*(TAN($C$44*((H6/($C$46*H13+$C$28))+$C$45)))+$C$47*H13+$C$48)/1000</f>
-        <v>439.08633867245737</v>
+        <f>($C$44+$C$45*(TAN($C$46*((H6/($C$48*H13+$C$28))+$C$47)))+$C$49*H13+$C$50)/1000</f>
+        <v>628.4325124094986</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>61</v>
@@ -1428,8 +1658,8 @@
         <v>69</v>
       </c>
       <c r="L15" s="8">
-        <f>($C$42+$C$43*(TAN($C$44*((L6/($C$46*L13+$C$28))+$C$45)))+$C$47*L13+$C$48)/1000</f>
-        <v>415.84472091981928</v>
+        <f>($C$44+$C$45*(TAN($C$46*((L6/($C$48*L13+$C$28))+$C$47)))+$C$49*L13+$C$50)/1000</f>
+        <v>438.61890270957446</v>
       </c>
       <c r="M15" s="9" t="s">
         <v>61</v>
@@ -1439,8 +1669,8 @@
         <v>69</v>
       </c>
       <c r="P15" s="8">
-        <f>($C$42+$C$43*(TAN($C$44*((P6/($C$46*P13+$C$28))+$C$45)))+$C$47*P13+$C$48)/1000</f>
-        <v>946.01537656198695</v>
+        <f>($C$44+$C$45*(TAN($C$46*((P6/($C$48*P13+$C$28))+$C$47)))+$C$49*P13+$C$50)/1000</f>
+        <v>150.75748358378104</v>
       </c>
       <c r="Q15" s="9" t="s">
         <v>61</v>
@@ -1449,14 +1679,34 @@
         <v>69</v>
       </c>
       <c r="T15" s="8">
-        <f>($C$42+$C$43*(TAN($C$44*((T6/($C$46*T13+$C$28))+$C$45)))+$C$47*T13+$C$48)/1000</f>
-        <v>203.64322637622598</v>
+        <f>($C$44+$C$45*(TAN($C$46*((T6/($C$48*T13+$C$28))+$C$47)))+$C$49*T13+$C$50)/1000</f>
+        <v>145.8392885878641</v>
       </c>
       <c r="U15" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="X15" s="8">
+        <f>($C$44+$C$45*(TAN($C$46*((X6/($C$48*X13+$C$28))+$C$47)))+$C$49*X13+$C$50)/1000</f>
+        <v>5411.8980974581154</v>
+      </c>
+      <c r="Y15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB15" s="8">
+        <f>($C$44+$C$45*(TAN($C$46*((AB6/($C$48*AB13+$C$28))+$C$47)))+$C$49*AB13+$C$50)/1000</f>
+        <v>5412.4759018545119</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1469,7 +1719,10 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="S16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA16" s="6" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1491,7 +1744,7 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1544,7 +1797,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1595,7 +1848,7 @@
       <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="12" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1653,7 +1906,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>105</v>
       </c>
       <c r="H31">
@@ -1691,7 +1944,7 @@
       <c r="D33" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1703,7 +1956,7 @@
         <v>45</v>
       </c>
       <c r="C34">
-        <v>2.2247430000000001</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -1714,30 +1967,32 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
       <c r="C36">
-        <v>2.1850000000000001E-2</v>
+        <f>7.9375/1000</f>
+        <v>7.9375000000000001E-3</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
         <v>51</v>
       </c>
       <c r="C37">
-        <v>2.555E-2</v>
+        <f>7.9375/1000</f>
+        <v>7.9375000000000001E-3</v>
       </c>
       <c r="D37" t="s">
         <v>16</v>
@@ -1746,13 +2001,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38">
-        <v>2.0639999999999999E-2</v>
+        <v>2.1850000000000001E-2</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
@@ -1760,157 +2015,189 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39">
-        <v>1.6080000000000001E-2</v>
+        <v>2.555E-2</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>2.0639999999999999E-2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="2">
-        <v>254300</v>
-      </c>
-      <c r="D42" t="s">
-        <v>71</v>
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41">
+        <v>1.6080000000000001E-2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="2">
-        <v>192000</v>
-      </c>
-      <c r="D43" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44">
-        <v>2.0265</v>
+        <v>60</v>
+      </c>
+      <c r="C44" s="2">
+        <v>254300</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45">
-        <v>-0.46100000000000002</v>
+        <v>62</v>
+      </c>
+      <c r="C45" s="2">
+        <v>192000</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="2">
-        <v>-3.3100000000000002E-4</v>
-      </c>
-      <c r="D46" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="C46">
+        <v>2.0265</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1230</v>
-      </c>
-      <c r="D47" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="C47">
+        <v>-0.46100000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C48" s="2">
-        <v>15600</v>
+        <v>-3.3100000000000002E-4</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1230</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50">
-        <v>620</v>
+        <v>68</v>
+      </c>
+      <c r="C50" s="2">
+        <v>15600</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53">
-        <v>0.48480000000000001</v>
-      </c>
-      <c r="D53" t="s">
-        <v>111</v>
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52">
+        <v>620</v>
+      </c>
+      <c r="D52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54">
-        <v>3.3059999999999999E-2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>62</v>
+      </c>
+      <c r="C55">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="C56">
+        <v>3.3059999999999999E-2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="G2:G3"/>

</xml_diff>

<commit_message>
Damped Hind Leg Updates
Damped Hing Leg Updates
</commit_message>
<xml_diff>
--- a/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Actuator Pressures Required to Move Joint Springs2.xlsx
+++ b/Code/Matlab/Analysis/DampedLeg_Krnacik/Haonan/Actuator Pressures Required to Move Joint Springs2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haonan\Documents\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\Code\Matlab\Analysis\DampedLeg_Krnacik\Haonan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD2D9D7-547C-47A0-90B5-9F1A0803CE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612E136-56E4-462D-A081-A113DD458BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -541,11 +541,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -578,6 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +648,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -690,7 +700,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -895,10 +905,10 @@
   <dimension ref="A1:AC60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="14" topLeftCell="Q18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1729,7 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="S16" s="18" t="s">
         <v>104</v>
       </c>
       <c r="AA16" s="6" t="s">
@@ -2194,18 +2204,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="S2:S3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>